<commit_message>
Added status to sampleworkbook
</commit_message>
<xml_diff>
--- a/LimsVisualizer/Samples/SampleWorkBook.xlsx
+++ b/LimsVisualizer/Samples/SampleWorkBook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="7290" windowWidth="28830" windowHeight="7350" activeTab="1"/>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="7305"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="7305" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meas Data" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
   <si>
     <t>Device Name:</t>
   </si>
@@ -235,13 +235,22 @@
   </si>
   <si>
     <t>Dummy Comment</t>
+  </si>
+  <si>
+    <t>SystemStatus</t>
+  </si>
+  <si>
+    <t>DeviceStatus</t>
+  </si>
+  <si>
+    <t>LineStatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,16 +266,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -341,20 +386,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,7 +731,7 @@
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26:AY26"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -4009,30 +4080,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4040,7 +4116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4048,7 +4124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4056,7 +4132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -4064,73 +4140,91 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="4" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>9999</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -4138,69 +4232,96 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>10000</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="3">
+      <c r="H9" s="3">
         <v>9.8540315628051793</v>
       </c>
-      <c r="F9" s="3">
+      <c r="I9" s="3">
         <v>10</v>
       </c>
-      <c r="G9" s="3">
+      <c r="J9" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>19999</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="3">
+      <c r="M10" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="K10" s="3">
+      <c r="N10" s="3">
         <v>1</v>
       </c>
-      <c r="L10" s="3">
+      <c r="O10" s="3">
         <v>1.0148130677545</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>20000</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -4208,69 +4329,96 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>29999</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="3">
+      <c r="H12" s="3">
         <v>9.8540315628051793</v>
       </c>
-      <c r="F12" s="3">
+      <c r="I12" s="3">
         <v>10</v>
       </c>
-      <c r="G12" s="3">
+      <c r="J12" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9">
+        <v>9999</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="3">
+      <c r="M13" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="K13" s="3">
+      <c r="N13" s="3">
         <v>1</v>
       </c>
-      <c r="L13" s="3">
+      <c r="O13" s="3">
         <v>1.0148130677545</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>0</v>
+      </c>
+      <c r="B14" s="10">
+        <v>10000</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4278,69 +4426,96 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>0</v>
+      </c>
+      <c r="B15" s="10">
+        <v>19999</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="3">
+      <c r="H15" s="3">
         <v>9.8540315628051793</v>
       </c>
-      <c r="F15" s="3">
+      <c r="I15" s="3">
         <v>10</v>
       </c>
-      <c r="G15" s="3">
+      <c r="J15" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>0</v>
+      </c>
+      <c r="B16" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="3">
+      <c r="M16" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="K16" s="3">
+      <c r="N16" s="3">
         <v>1</v>
       </c>
-      <c r="L16" s="3">
+      <c r="O16" s="3">
         <v>1.0148130677545</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>0</v>
+      </c>
+      <c r="B17" s="11">
+        <v>29999</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -4348,69 +4523,96 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>0</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="9">
+        <v>9999</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="3">
+      <c r="H18" s="3">
         <v>9.8540315628051793</v>
       </c>
-      <c r="F18" s="3">
+      <c r="I18" s="3">
         <v>10</v>
       </c>
-      <c r="G18" s="3">
+      <c r="J18" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>0</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>10000</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="3">
+      <c r="M19" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="K19" s="3">
+      <c r="N19" s="3">
         <v>1</v>
       </c>
-      <c r="L19" s="3">
+      <c r="O19" s="3">
         <v>1.0148130677545</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>0</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>19999</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -4418,60 +4620,86 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>0</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11">
+        <v>20000</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="3">
+      <c r="H21" s="3">
         <v>9.8540315628051793</v>
       </c>
-      <c r="F21" s="3">
+      <c r="I21" s="3">
         <v>10</v>
       </c>
-      <c r="G21" s="3">
+      <c r="J21" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>0</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11">
+        <v>29999</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J22" s="3">
+      <c r="M22" s="3">
         <v>-0.145968437194824</v>
       </c>
-      <c r="K22" s="3">
+      <c r="N22" s="3">
         <v>1</v>
       </c>
-      <c r="L22" s="3">
+      <c r="O22" s="3">
         <v>1.0148130677545</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="K6:O6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>